<commit_message>
IMM instrument Id SGD JPY
</commit_message>
<xml_diff>
--- a/db/IMM_InstrumentId_Convention.xlsx
+++ b/db/IMM_InstrumentId_Convention.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\csv-to-db\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDCBDE2-B837-4CDD-AB11-BD29C1DF8A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F62ABD-7713-4817-B88A-4213627B927E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SGD-6M" sheetId="1" r:id="rId1"/>
     <sheet name="SGD-SORA-IMM" sheetId="2" r:id="rId2"/>
-    <sheet name="TONA-STD-IMM" sheetId="3" r:id="rId3"/>
-    <sheet name="TONA-IMM" sheetId="4" r:id="rId4"/>
+    <sheet name="TONA-STD" sheetId="5" r:id="rId3"/>
+    <sheet name="TONA-IMM" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>Tenor</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>TONA</t>
+  </si>
+  <si>
+    <t>OY0</t>
+  </si>
+  <si>
+    <t>Prefix-Except-Front-Contract</t>
+  </si>
+  <si>
+    <t>OYM</t>
   </si>
 </sst>
 </file>
@@ -393,7 +402,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +624,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="I17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,380 +992,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C3CD04-F15E-4DB5-992A-30D5998F26B5}">
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>44916</v>
-      </c>
-      <c r="C1" s="1">
-        <v>45000</v>
-      </c>
-      <c r="D1" s="1">
-        <v>45098</v>
-      </c>
-      <c r="E1" s="1">
-        <v>45189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
-        <v>OYS0101YTONA</v>
-      </c>
-      <c r="C2" t="str">
-        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
-        <v>OYS0201YTONA</v>
-      </c>
-      <c r="D2" t="str">
-        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
-        <v>OYS0301YTONA</v>
-      </c>
-      <c r="E2" t="str">
-        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
-        <v>OYS0401YTONA</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B16" si="0">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
-        <v>OYS0102YTONA</v>
-      </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C16" si="1">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
-        <v>OYS0202YTONA</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D16" si="2">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
-        <v>OYS0302YTONA</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E16" si="3">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
-        <v>OYS0402YTONA</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0103YTONA</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0203YTONA</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0303YTONA</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0403YTONA</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0104YTONA</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0204YTONA</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0304YTONA</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0404YTONA</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0105YTONA</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0205YTONA</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0305YTONA</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0405YTONA</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0106YTONA</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0206YTONA</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0306YTONA</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0406YTONA</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0107YTONA</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0207YTONA</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0307YTONA</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0407YTONA</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0108YTONA</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0208YTONA</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0308YTONA</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0408YTONA</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0109YTONA</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0209YTONA</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0309YTONA</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0409YTONA</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0110YTONA</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0210YTONA</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0310YTONA</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0410YTONA</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0112YTONA</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0212YTONA</v>
-      </c>
-      <c r="D12" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0312YTONA</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0412YTONA</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>15</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0115YTONA</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0215YTONA</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0315YTONA</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0415YTONA</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>20</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0120YTONA</v>
-      </c>
-      <c r="C14" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0220YTONA</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0320YTONA</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0420YTONA</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>25</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0125YTONA</v>
-      </c>
-      <c r="C15" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0225YTONA</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0325YTONA</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0425YTONA</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>30</v>
-      </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>OYS0130YTONA</v>
-      </c>
-      <c r="C16" t="str">
-        <f t="shared" si="1"/>
-        <v>OYS0230YTONA</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="2"/>
-        <v>OYS0330YTONA</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="3"/>
-        <v>OYS0430YTONA</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8756B30-4EAC-4944-A678-B6942010A7EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27DE306-A9F8-40E3-8BF6-16F0E1271F62}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,6 +1005,7 @@
     <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1390,19 +1031,19 @@
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
-        <v>OGS0101YSORA</v>
+        <v>OYS0101YTONA</v>
       </c>
       <c r="C2" t="str">
         <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
-        <v>OGS0201YSORA</v>
+        <v>OYS0201YTONA</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
-        <v>OGS0301YSORA</v>
+        <v>OYS0301YTONA</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
-        <v>OGS0401YSORA</v>
+        <v>OYS0401YTONA</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1411,19 +1052,19 @@
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B16" si="0">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
-        <v>OGS0102YSORA</v>
+        <v>OYS0102YTONA</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C16" si="1">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
-        <v>OGS0202YSORA</v>
+        <v>OYS0202YTONA</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D16" si="2">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
-        <v>OGS0302YSORA</v>
+        <v>OYS0302YTONA</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E16" si="3">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
-        <v>OGS0402YSORA</v>
+        <v>OYS0402YTONA</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1432,19 +1073,19 @@
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0103YSORA</v>
+        <v>OYS0103YTONA</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0203YSORA</v>
+        <v>OYS0203YTONA</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0303YSORA</v>
+        <v>OYS0303YTONA</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0403YSORA</v>
+        <v>OYS0403YTONA</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1453,19 +1094,19 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0104YSORA</v>
+        <v>OYS0104YTONA</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0204YSORA</v>
+        <v>OYS0204YTONA</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0304YSORA</v>
+        <v>OYS0304YTONA</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0404YSORA</v>
+        <v>OYS0404YTONA</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1474,19 +1115,19 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0105YSORA</v>
+        <v>OYS0105YTONA</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0205YSORA</v>
+        <v>OYS0205YTONA</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0305YSORA</v>
+        <v>OYS0305YTONA</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0405YSORA</v>
+        <v>OYS0405YTONA</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1495,19 +1136,19 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0106YSORA</v>
+        <v>OYS0106YTONA</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0206YSORA</v>
+        <v>OYS0206YTONA</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0306YSORA</v>
+        <v>OYS0306YTONA</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0406YSORA</v>
+        <v>OYS0406YTONA</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1516,19 +1157,19 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0107YSORA</v>
+        <v>OYS0107YTONA</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0207YSORA</v>
+        <v>OYS0207YTONA</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0307YSORA</v>
+        <v>OYS0307YTONA</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0407YSORA</v>
+        <v>OYS0407YTONA</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1537,19 +1178,19 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0108YSORA</v>
+        <v>OYS0108YTONA</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0208YSORA</v>
+        <v>OYS0208YTONA</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0308YSORA</v>
+        <v>OYS0308YTONA</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0408YSORA</v>
+        <v>OYS0408YTONA</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1558,19 +1199,19 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0109YSORA</v>
+        <v>OYS0109YTONA</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0209YSORA</v>
+        <v>OYS0209YTONA</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0309YSORA</v>
+        <v>OYS0309YTONA</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0409YSORA</v>
+        <v>OYS0409YTONA</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1579,19 +1220,19 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0110YSORA</v>
+        <v>OYS0110YTONA</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0210YSORA</v>
+        <v>OYS0210YTONA</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0310YSORA</v>
+        <v>OYS0310YTONA</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0410YSORA</v>
+        <v>OYS0410YTONA</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1600,19 +1241,19 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0112YSORA</v>
+        <v>OYS0112YTONA</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0212YSORA</v>
+        <v>OYS0212YTONA</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0312YSORA</v>
+        <v>OYS0312YTONA</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0412YSORA</v>
+        <v>OYS0412YTONA</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1621,19 +1262,19 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0115YSORA</v>
+        <v>OYS0115YTONA</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0215YSORA</v>
+        <v>OYS0215YTONA</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0315YSORA</v>
+        <v>OYS0315YTONA</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0415YSORA</v>
+        <v>OYS0415YTONA</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1642,19 +1283,19 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0120YSORA</v>
+        <v>OYS0120YTONA</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0220YSORA</v>
+        <v>OYS0220YTONA</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0320YSORA</v>
+        <v>OYS0320YTONA</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0420YSORA</v>
+        <v>OYS0420YTONA</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1663,19 +1304,19 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0125YSORA</v>
+        <v>OYS0125YTONA</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0225YSORA</v>
+        <v>OYS0225YTONA</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0325YSORA</v>
+        <v>OYS0325YTONA</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0425YSORA</v>
+        <v>OYS0425YTONA</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1684,19 +1325,19 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>OGS0130YSORA</v>
+        <v>OYS0130YTONA</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
-        <v>OGS0230YSORA</v>
+        <v>OYS0230YTONA</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="2"/>
-        <v>OGS0330YSORA</v>
+        <v>OYS0330YTONA</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="3"/>
-        <v>OGS0430YSORA</v>
+        <v>OYS0430YTONA</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1704,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1712,7 +1353,385 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C3CD04-F15E-4DB5-992A-30D5998F26B5}">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>44916</v>
+      </c>
+      <c r="C1" s="1">
+        <v>45000</v>
+      </c>
+      <c r="D1" s="1">
+        <v>45098</v>
+      </c>
+      <c r="E1" s="1">
+        <v>45189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>CONCATENATE($B$19,  TEXT(COLUMN()-2,REPT("0",2)),"12M",$B$20)</f>
+        <v>OY00012MTONA</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE($B$21,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>OYM0201YTONA</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE($B$21,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>OYM0301YTONA</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE($B$21,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>OYM0401YTONA</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>CONCATENATE($B$19,  TEXT(COLUMN()-2,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>OY00002YTONA</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C16" si="0">CONCATENATE($B$21,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>OYM0202YTONA</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D16" si="1">CONCATENATE($B$21,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>OYM0302YTONA</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E16" si="2">CONCATENATE($B$21,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>OYM0402YTONA</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B16" si="3">CONCATENATE($B$19,  TEXT(COLUMN()-2,REPT("0",2)),TEXT(A4,REPT("0",2)), "Y",$B$20)</f>
+        <v>OY00003YTONA</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0203YTONA</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0303YTONA</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0403YTONA</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00004YTONA</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0204YTONA</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0304YTONA</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0404YTONA</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00005YTONA</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0205YTONA</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0305YTONA</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0405YTONA</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00006YTONA</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0206YTONA</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0306YTONA</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0406YTONA</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00007YTONA</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0207YTONA</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0307YTONA</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0407YTONA</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00008YTONA</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0208YTONA</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0308YTONA</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0408YTONA</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00009YTONA</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0209YTONA</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0309YTONA</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0409YTONA</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00010YTONA</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0210YTONA</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0310YTONA</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0410YTONA</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00012YTONA</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0212YTONA</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0312YTONA</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0412YTONA</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00015YTONA</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0215YTONA</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0315YTONA</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0415YTONA</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00020YTONA</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0220YTONA</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0320YTONA</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0420YTONA</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>25</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00025YTONA</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0225YTONA</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0325YTONA</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0425YTONA</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="3"/>
+        <v>OY00030YTONA</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>OYM0230YTONA</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>OYM0330YTONA</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="2"/>
+        <v>OYM0430YTONA</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IMM instrument Id SGD JPY AUD HKD
</commit_message>
<xml_diff>
--- a/db/IMM_InstrumentId_Convention.xlsx
+++ b/db/IMM_InstrumentId_Convention.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\csv-to-db\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F62ABD-7713-4817-B88A-4213627B927E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B36AFBA-F312-4764-B643-C3246BA078CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SGD-6M" sheetId="1" r:id="rId1"/>
     <sheet name="SGD-SORA-IMM" sheetId="2" r:id="rId2"/>
     <sheet name="TONA-STD" sheetId="5" r:id="rId3"/>
     <sheet name="TONA-IMM" sheetId="3" r:id="rId4"/>
+    <sheet name="AUD-IMM-3M" sheetId="6" r:id="rId5"/>
+    <sheet name="AUD-IMM-6M" sheetId="7" r:id="rId6"/>
+    <sheet name="HKD-IMM" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Tenor</t>
   </si>
@@ -73,13 +76,28 @@
   <si>
     <t>OYM</t>
   </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>A3MQ</t>
+  </si>
+  <si>
+    <t>A6MS</t>
+  </si>
+  <si>
+    <t>RKM</t>
+  </si>
+  <si>
+    <t>H3MQ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -118,7 +136,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,19 +453,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" ref="B2:B9" si="0">CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
         <v>RGM0101YS6MS</v>
       </c>
       <c r="C2" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" ref="C2:C9" si="1">CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
         <v>RGM0201YS6MS</v>
       </c>
       <c r="D2" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" ref="D2:D9" si="2">CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
         <v>RGM0301YS6MS</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" ref="E2:E9" si="3">CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
         <v>RGM0401YS6MS</v>
       </c>
     </row>
@@ -456,19 +474,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="0"/>
         <v>RGM0102YS6MS</v>
       </c>
       <c r="C3" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="1"/>
         <v>RGM0202YS6MS</v>
       </c>
       <c r="D3" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="2"/>
         <v>RGM0302YS6MS</v>
       </c>
       <c r="E3" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="3"/>
         <v>RGM0402YS6MS</v>
       </c>
     </row>
@@ -477,19 +495,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A4,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="0"/>
         <v>RGM0103YS6MS</v>
       </c>
       <c r="C4" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A4,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="1"/>
         <v>RGM0203YS6MS</v>
       </c>
       <c r="D4" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A4,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="2"/>
         <v>RGM0303YS6MS</v>
       </c>
       <c r="E4" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A4,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="3"/>
         <v>RGM0403YS6MS</v>
       </c>
     </row>
@@ -498,19 +516,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A5,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="0"/>
         <v>RGM0104YS6MS</v>
       </c>
       <c r="C5" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A5,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="1"/>
         <v>RGM0204YS6MS</v>
       </c>
       <c r="D5" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A5,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="2"/>
         <v>RGM0304YS6MS</v>
       </c>
       <c r="E5" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A5,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="3"/>
         <v>RGM0404YS6MS</v>
       </c>
     </row>
@@ -519,19 +537,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A6,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="0"/>
         <v>RGM0105YS6MS</v>
       </c>
       <c r="C6" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A6,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="1"/>
         <v>RGM0205YS6MS</v>
       </c>
       <c r="D6" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A6,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="2"/>
         <v>RGM0305YS6MS</v>
       </c>
       <c r="E6" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A6,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="3"/>
         <v>RGM0405YS6MS</v>
       </c>
     </row>
@@ -540,19 +558,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A7,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="0"/>
         <v>RGM0106YS6MS</v>
       </c>
       <c r="C7" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A7,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="1"/>
         <v>RGM0206YS6MS</v>
       </c>
       <c r="D7" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A7,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="2"/>
         <v>RGM0306YS6MS</v>
       </c>
       <c r="E7" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A7,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="3"/>
         <v>RGM0406YS6MS</v>
       </c>
     </row>
@@ -561,19 +579,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A8,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="0"/>
         <v>RGM0107YS6MS</v>
       </c>
       <c r="C8" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A8,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="1"/>
         <v>RGM0207YS6MS</v>
       </c>
       <c r="D8" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A8,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="2"/>
         <v>RGM0307YS6MS</v>
       </c>
       <c r="E8" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A8,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="3"/>
         <v>RGM0407YS6MS</v>
       </c>
     </row>
@@ -582,19 +600,19 @@
         <v>10</v>
       </c>
       <c r="B9" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A9,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="0"/>
         <v>RGM0110YS6MS</v>
       </c>
       <c r="C9" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A9,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="1"/>
         <v>RGM0210YS6MS</v>
       </c>
       <c r="D9" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A9,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="2"/>
         <v>RGM0310YS6MS</v>
       </c>
       <c r="E9" t="str">
-        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A9,REPT("0",2)), "Y",$B$13)</f>
+        <f t="shared" si="3"/>
         <v>RGM0410YS6MS</v>
       </c>
     </row>
@@ -995,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27DE306-A9F8-40E3-8BF6-16F0E1271F62}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1737,4 +1755,968 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C030B1-EB6E-43A1-B7B2-2ED07900C415}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>44916</v>
+      </c>
+      <c r="C1" s="1">
+        <v>45000</v>
+      </c>
+      <c r="D1" s="1">
+        <v>45098</v>
+      </c>
+      <c r="E1" s="1">
+        <v>45189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0101YA3MQ</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0201YA3MQ</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0301YA3MQ</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0401YA3MQ</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B16" si="0">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0102YA3MQ</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C16" si="1">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0202YA3MQ</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D16" si="2">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0302YA3MQ</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E16" si="3">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0402YA3MQ</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0103YA3MQ</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0203YA3MQ</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0303YA3MQ</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0403YA3MQ</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0104YA3MQ</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0204YA3MQ</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0304YA3MQ</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0404YA3MQ</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0105YA3MQ</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0205YA3MQ</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0305YA3MQ</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0405YA3MQ</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0106YA3MQ</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0206YA3MQ</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0306YA3MQ</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0406YA3MQ</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0107YA3MQ</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0207YA3MQ</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0307YA3MQ</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0407YA3MQ</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0108YA3MQ</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0208YA3MQ</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0308YA3MQ</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0408YA3MQ</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0109YA3MQ</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0209YA3MQ</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0309YA3MQ</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0409YA3MQ</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0110YA3MQ</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0210YA3MQ</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0310YA3MQ</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0410YA3MQ</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0112YA3MQ</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0212YA3MQ</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0312YA3MQ</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0412YA3MQ</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0115YA3MQ</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0215YA3MQ</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0315YA3MQ</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0415YA3MQ</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0120YA3MQ</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0220YA3MQ</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0320YA3MQ</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0420YA3MQ</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>25</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0125YA3MQ</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0225YA3MQ</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0325YA3MQ</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0425YA3MQ</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0130YA3MQ</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0230YA3MQ</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0330YA3MQ</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0430YA3MQ</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72D7102F-384F-4028-A1F1-4FEE77679E09}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>44916</v>
+      </c>
+      <c r="C1" s="1">
+        <v>45000</v>
+      </c>
+      <c r="D1" s="1">
+        <v>45098</v>
+      </c>
+      <c r="E1" s="1">
+        <v>45189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0101YA6MS</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0201YA6MS</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0301YA6MS</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0401YA6MS</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B16" si="0">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0102YA6MS</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C16" si="1">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0202YA6MS</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D16" si="2">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0302YA6MS</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E16" si="3">CONCATENATE($B$19,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$20)</f>
+        <v>RAM0402YA6MS</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0103YA6MS</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0203YA6MS</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0303YA6MS</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0403YA6MS</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0104YA6MS</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0204YA6MS</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0304YA6MS</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0404YA6MS</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0105YA6MS</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0205YA6MS</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0305YA6MS</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0405YA6MS</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0106YA6MS</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0206YA6MS</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0306YA6MS</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0406YA6MS</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0107YA6MS</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0207YA6MS</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0307YA6MS</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0407YA6MS</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0108YA6MS</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0208YA6MS</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0308YA6MS</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0408YA6MS</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0109YA6MS</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0209YA6MS</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0309YA6MS</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0409YA6MS</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0110YA6MS</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0210YA6MS</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0310YA6MS</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0410YA6MS</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0112YA6MS</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0212YA6MS</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0312YA6MS</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0412YA6MS</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0115YA6MS</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0215YA6MS</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0315YA6MS</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0415YA6MS</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0120YA6MS</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0220YA6MS</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0320YA6MS</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0420YA6MS</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>25</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0125YA6MS</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0225YA6MS</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0325YA6MS</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0425YA6MS</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>RAM0130YA6MS</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v>RAM0230YA6MS</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="2"/>
+        <v>RAM0330YA6MS</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="3"/>
+        <v>RAM0430YA6MS</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D5F8AD-1612-493B-A1CC-0B993C3D3B95}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>44916</v>
+      </c>
+      <c r="C1" s="1">
+        <v>45000</v>
+      </c>
+      <c r="D1" s="1">
+        <v>45098</v>
+      </c>
+      <c r="E1" s="1">
+        <v>45189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0101YH3MQ</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0201YH3MQ</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0301YH3MQ</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A2,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0401YH3MQ</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0102YH3MQ</v>
+      </c>
+      <c r="C3" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0202YH3MQ</v>
+      </c>
+      <c r="D3" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0302YH3MQ</v>
+      </c>
+      <c r="E3" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A3,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0402YH3MQ</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A4,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0103YH3MQ</v>
+      </c>
+      <c r="C4" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A4,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0203YH3MQ</v>
+      </c>
+      <c r="D4" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A4,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0303YH3MQ</v>
+      </c>
+      <c r="E4" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A4,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0403YH3MQ</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A5,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0104YH3MQ</v>
+      </c>
+      <c r="C5" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A5,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0204YH3MQ</v>
+      </c>
+      <c r="D5" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A5,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0304YH3MQ</v>
+      </c>
+      <c r="E5" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A5,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0404YH3MQ</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A6,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0105YH3MQ</v>
+      </c>
+      <c r="C6" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A6,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0205YH3MQ</v>
+      </c>
+      <c r="D6" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A6,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0305YH3MQ</v>
+      </c>
+      <c r="E6" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A6,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0405YH3MQ</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A7,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0106YH3MQ</v>
+      </c>
+      <c r="C7" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A7,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0206YH3MQ</v>
+      </c>
+      <c r="D7" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A7,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0306YH3MQ</v>
+      </c>
+      <c r="E7" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A7,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0406YH3MQ</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A8,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0107YH3MQ</v>
+      </c>
+      <c r="C8" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A8,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0207YH3MQ</v>
+      </c>
+      <c r="D8" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A8,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0307YH3MQ</v>
+      </c>
+      <c r="E8" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A8,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0407YH3MQ</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A9,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0110YH3MQ</v>
+      </c>
+      <c r="C9" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A9,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0210YH3MQ</v>
+      </c>
+      <c r="D9" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A9,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0310YH3MQ</v>
+      </c>
+      <c r="E9" t="str">
+        <f>CONCATENATE($B$12,  TEXT(COLUMN()-1,REPT("0",2)),TEXT(A9,REPT("0",2)), "Y",$B$13)</f>
+        <v>RKM0410YH3MQ</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>